<commit_message>
Update xcel and testng files
</commit_message>
<xml_diff>
--- a/Testdata/GMTestData.xlsx
+++ b/Testdata/GMTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="630" windowWidth="14535" windowHeight="2445" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="630" windowWidth="14535" windowHeight="5385" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="PackageCouponCodes" sheetId="22" r:id="rId1"/>
@@ -16,22 +16,28 @@
     <sheet name="Scheduled" sheetId="20" r:id="rId7"/>
     <sheet name="CarDetails" sheetId="8" r:id="rId8"/>
     <sheet name="CityLocation" sheetId="14" r:id="rId9"/>
-    <sheet name="Checkout" sheetId="7" r:id="rId10"/>
-    <sheet name="Careers" sheetId="15" r:id="rId11"/>
-    <sheet name="CheckoutAddMoreWheelCare" sheetId="10" r:id="rId12"/>
-    <sheet name="CheckoutAddMoreScheduledService" sheetId="12" r:id="rId13"/>
-    <sheet name="Periodic Service" sheetId="23" r:id="rId14"/>
-    <sheet name="AC Service" sheetId="24" r:id="rId15"/>
-    <sheet name="Batteries" sheetId="25" r:id="rId16"/>
-    <sheet name="LightAndFitment" sheetId="26" r:id="rId17"/>
-    <sheet name="CheckoutAddMoreDentingService" sheetId="11" r:id="rId18"/>
-    <sheet name="CheckoutAddMoreCarCareService" sheetId="13" r:id="rId19"/>
-    <sheet name="RequestCallBack" sheetId="1" r:id="rId20"/>
-    <sheet name="Practice" sheetId="5" r:id="rId21"/>
-    <sheet name="Login" sheetId="9" r:id="rId22"/>
+    <sheet name="TyresAndWheelCare" sheetId="29" r:id="rId10"/>
+    <sheet name="InsuranceClaim" sheetId="30" r:id="rId11"/>
+    <sheet name="DetailingServices" sheetId="31" r:id="rId12"/>
+    <sheet name="CustomServices" sheetId="32" r:id="rId13"/>
+    <sheet name="WindSheildsAndGlass" sheetId="33" r:id="rId14"/>
+    <sheet name="Checkout" sheetId="7" r:id="rId15"/>
+    <sheet name="CarSpaAndCleaning" sheetId="27" r:id="rId16"/>
+    <sheet name="Careers" sheetId="15" r:id="rId17"/>
+    <sheet name="CheckoutAddMoreWheelCare" sheetId="10" r:id="rId18"/>
+    <sheet name="CheckoutAddMoreScheduledService" sheetId="12" r:id="rId19"/>
+    <sheet name="Periodic Service" sheetId="23" r:id="rId20"/>
+    <sheet name="AC Service" sheetId="24" r:id="rId21"/>
+    <sheet name="Batteries" sheetId="25" r:id="rId22"/>
+    <sheet name="LightAndFitment" sheetId="26" r:id="rId23"/>
+    <sheet name="CheckoutAddMoreDentingService" sheetId="11" r:id="rId24"/>
+    <sheet name="CheckoutAddMoreCarCareService" sheetId="13" r:id="rId25"/>
+    <sheet name="RequestCallBack" sheetId="1" r:id="rId26"/>
+    <sheet name="Practice" sheetId="5" r:id="rId27"/>
+    <sheet name="Login" sheetId="9" r:id="rId28"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I6"/>
+  <oleSize ref="A1:M15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="266">
   <si>
     <t>Honda</t>
   </si>
@@ -379,21 +385,6 @@
     <t>PlanName</t>
   </si>
   <si>
-    <t>BONNET</t>
-  </si>
-  <si>
-    <t>FRONT BUMPER</t>
-  </si>
-  <si>
-    <t>REAR BUMPER</t>
-  </si>
-  <si>
-    <t>TRUNK</t>
-  </si>
-  <si>
-    <t>FULL BODY</t>
-  </si>
-  <si>
     <t>Thane</t>
   </si>
   <si>
@@ -791,6 +782,69 @@
   </si>
   <si>
     <t>Front Headlight</t>
+  </si>
+  <si>
+    <t>Denting &amp; Painting</t>
+  </si>
+  <si>
+    <t>Whole Body</t>
+  </si>
+  <si>
+    <t>Full Body Dent Paint</t>
+  </si>
+  <si>
+    <t>Car Spa &amp; Cleaning</t>
+  </si>
+  <si>
+    <t>Car Interior Spa</t>
+  </si>
+  <si>
+    <t>Cleaning &amp; Inspection</t>
+  </si>
+  <si>
+    <t>Tyres &amp; Wheel Care</t>
+  </si>
+  <si>
+    <t>Tyres Replacement</t>
+  </si>
+  <si>
+    <t>Michelin Primacy 3ZP</t>
+  </si>
+  <si>
+    <t>Insurance Claims</t>
+  </si>
+  <si>
+    <t>Accidental Repairs</t>
+  </si>
+  <si>
+    <t>Doorstep Accidental Inspection</t>
+  </si>
+  <si>
+    <t>Detailing Services</t>
+  </si>
+  <si>
+    <t>Detailing &amp; Coatings</t>
+  </si>
+  <si>
+    <t>PPF - Paint Protection Film</t>
+  </si>
+  <si>
+    <t>Custom Services</t>
+  </si>
+  <si>
+    <t>Inspection</t>
+  </si>
+  <si>
+    <t>Engine Scanning</t>
+  </si>
+  <si>
+    <t>Windshields &amp; Glass</t>
+  </si>
+  <si>
+    <t>Glasses</t>
+  </si>
+  <si>
+    <t>Front Windshield Replacement</t>
   </si>
 </sst>
 </file>
@@ -1281,167 +1335,167 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1451,9 +1505,222 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1517,16 +1784,16 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E2" s="4">
         <v>9770674475</v>
@@ -1544,7 +1811,7 @@
         <v>64</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>13</v>
@@ -1561,10 +1828,10 @@
         <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1585,7 +1852,7 @@
         <v>65</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -1626,7 +1893,7 @@
         <v>63</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>15</v>
@@ -1647,7 +1914,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1690,7 +2000,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>108</v>
@@ -1702,7 +2012,7 @@
         <v>9999999999</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,7 +2032,7 @@
         <v>9999999999</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1742,7 +2052,7 @@
         <v>9999999999</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1762,7 +2072,7 @@
         <v>9999999999</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1782,7 +2092,7 @@
         <v>9999999999</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1796,7 +2106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -1896,7 +2206,7 @@
         <v>65</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>14</v>
@@ -1940,7 +2250,7 @@
         <v>63</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>15</v>
@@ -1961,7 +2271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
@@ -2061,7 +2371,7 @@
         <v>64</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>13</v>
@@ -2105,7 +2415,7 @@
         <v>65</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>14</v>
@@ -2149,7 +2459,7 @@
         <v>63</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>15</v>
@@ -2193,7 +2503,7 @@
         <v>95</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>16</v>
@@ -2215,7 +2525,204 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2232,64 +2739,64 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" t="s">
         <v>224</v>
-      </c>
-      <c r="B3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2298,12 +2805,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2316,25 +2823,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2343,7 +2850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2360,24 +2867,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2386,7 +2893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2403,24 +2910,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +2936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -2529,7 +3036,7 @@
         <v>64</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>13</v>
@@ -2573,7 +3080,7 @@
         <v>63</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>15</v>
@@ -2617,7 +3124,7 @@
         <v>95</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>16</v>
@@ -2639,7 +3146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -2739,7 +3246,7 @@
         <v>65</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>14</v>
@@ -2783,7 +3290,7 @@
         <v>63</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>15</v>
@@ -2827,7 +3334,7 @@
         <v>95</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>16</v>
@@ -2849,204 +3356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -3083,10 +3393,10 @@
         <v>7</v>
       </c>
       <c r="F1" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>205</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>210</v>
       </c>
       <c r="H1" s="22" t="s">
         <v>103</v>
@@ -3109,10 +3419,10 @@
         <v>9999999999</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>109</v>
@@ -3135,10 +3445,10 @@
         <v>9999999999</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>109</v>
@@ -3161,10 +3471,10 @@
         <v>9999999999</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>109</v>
@@ -3187,10 +3497,10 @@
         <v>9999999999</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>214</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>109</v>
@@ -3213,10 +3523,10 @@
         <v>9999999999</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>109</v>
@@ -3233,7 +3543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
@@ -3617,7 +3927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3637,7 +3947,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>91</v>
@@ -3651,7 +3961,7 @@
         <v>8919345081</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3687,7 +3997,7 @@
         <v>101</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>61</v>
@@ -3696,7 +4006,7 @@
         <v>91</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3707,16 +4017,16 @@
         <v>108</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D2" s="4">
         <v>8919345081</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3934,7 +4244,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>85</v>
@@ -3980,10 +4290,10 @@
         <v>61</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3991,16 +4301,16 @@
         <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C2" s="15">
         <v>9999999999</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -4013,7 +4323,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4021,112 +4331,34 @@
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>229</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4178,7 +4410,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4195,7 +4427,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4212,7 +4444,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4483,12 +4715,12 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>